<commit_message>
Added a graph. Need to fix x axis.
</commit_message>
<xml_diff>
--- a/Exempel.xlsx
+++ b/Exempel.xlsx
@@ -16,22 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>Input:</t>
-  </si>
-  <si>
-    <t>Amorterings modell</t>
-  </si>
-  <si>
-    <t>Nivå 1:</t>
-  </si>
-  <si>
-    <t>Nivå 2:</t>
-  </si>
-  <si>
-    <t>Möjlighet att lägga till fler</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Ränta:</t>
   </si>
@@ -48,9 +33,6 @@
     <t>100kr</t>
   </si>
   <si>
-    <t>Ränteavdrag: 30%</t>
-  </si>
-  <si>
     <t>Output:</t>
   </si>
   <si>
@@ -88,6 +70,30 @@
   </si>
   <si>
     <t>Gör en user control. Kanske kan utöka med fler beräkningar senare</t>
+  </si>
+  <si>
+    <t>Amortizing model</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>Level 2</t>
+  </si>
+  <si>
+    <t>Add level</t>
+  </si>
+  <si>
+    <t>Down to:</t>
+  </si>
+  <si>
+    <t>Amortization amount per year</t>
+  </si>
+  <si>
+    <t>Loan &amp; Capital:</t>
+  </si>
+  <si>
+    <t>Interest deduction</t>
   </si>
 </sst>
 </file>
@@ -428,35 +434,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="27.26171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1">
         <v>0.7</v>
@@ -465,9 +478,9 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1">
         <v>0.5</v>
@@ -476,88 +489,91 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B13" s="2">
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>